<commit_message>
array min max solved
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CHROME_DOWNLOAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B9960B-FF0B-4B28-A6E0-1C92FB815080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2AE6BD-B289-4626-9C64-F641827AB21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2755,7 +2755,7 @@
     <col min="10" max="10" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="48" t="s">
         <v>3</v>
       </c>
@@ -2950,7 +2950,9 @@
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D7" s="40" t="s">
         <v>699</v>
       </c>
@@ -33207,21 +33209,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{5F4E176D-2B93-46A0-950B-B26013ED7CB4}"/>
+      <autoFilter ref="A293:C332" xr:uid="{03B760BD-3098-4200-A88B-7DD87E81F132}"/>
+    </customSheetView>
+    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{0334D6A3-DE11-4DD4-B6A9-A1816B2D57A8}"/>
     </customSheetView>
     <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{BC8C5B64-2EEE-45C8-9C1B-CC9C88804F96}"/>
+      <autoFilter ref="A11:D37" xr:uid="{D1B03329-67BB-449A-9C63-03D046BFC734}"/>
     </customSheetView>
-    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{D23E26D8-230C-405D-B29D-DE30340E0E86}"/>
-    </customSheetView>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{CB1E0578-1BFA-4B6B-B9DC-741C10683B95}"/>
+      <autoFilter ref="A11:C37" xr:uid="{ACB31813-514A-451D-A887-2292A5F85160}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -33650,12 +33652,12 @@
       <c r="B4" s="50"/>
       <c r="C4" s="50"/>
     </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A5" s="9"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -33664,7 +33666,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -33673,7 +33675,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -33682,7 +33684,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A9" s="9"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>

</xml_diff>

<commit_message>
array buy and sell stock
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400EBE1B-6D24-4FCE-8420-429C10F1D5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2841F8-EB6F-40F8-B151-FB0D1AD6A21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,8 +2739,8 @@
   </sheetPr>
   <dimension ref="A1:AC914"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3233,7 +3233,9 @@
       <c r="B14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D14" s="40" t="s">
         <v>699</v>
       </c>
@@ -33215,21 +33217,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{71C16F06-0CC9-47C5-B1BA-67B450363717}"/>
+      <autoFilter ref="A293:C332" xr:uid="{9A2F6395-0EA6-4E31-B978-BE1D00437761}"/>
+    </customSheetView>
+    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{D8543D54-261E-426C-847B-814C8CD4A274}"/>
     </customSheetView>
     <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{4FF1D1B8-F76D-4302-B74B-38277B55892E}"/>
+      <autoFilter ref="A11:D37" xr:uid="{3CFF4FB4-495E-4982-B059-C6B847B23D58}"/>
     </customSheetView>
-    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{94B0E5C7-16A1-41CC-A3B0-593620B26B60}"/>
-    </customSheetView>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{8F45A950-5A37-447A-A3FB-AFA83CE32034}"/>
+      <autoFilter ref="A11:C37" xr:uid="{96B3A945-FB99-402E-AFD9-475201AF1BD3}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
trapped rainwater and maxsubarray product
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2841F8-EB6F-40F8-B151-FB0D1AD6A21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFA6185-F996-4646-B5C2-C979B874B5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,8 +2739,8 @@
   </sheetPr>
   <dimension ref="A1:AC914"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3352,7 +3352,9 @@
       <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D17" s="40" t="s">
         <v>699</v>
       </c>
@@ -3432,7 +3434,9 @@
       <c r="B19" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D19" s="40" t="s">
         <v>699</v>
       </c>
@@ -33217,21 +33221,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{9A2F6395-0EA6-4E31-B978-BE1D00437761}"/>
+      <autoFilter ref="A11:C37" xr:uid="{AA339591-1250-46F1-A629-591C44240F05}"/>
+    </customSheetView>
+    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{9C473676-C4E1-4CBD-8AA3-2A3E76780763}"/>
     </customSheetView>
     <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{D8543D54-261E-426C-847B-814C8CD4A274}"/>
+      <autoFilter ref="A11:D37" xr:uid="{13E6EA58-A3C6-438A-9C99-AA00D7C85D36}"/>
     </customSheetView>
-    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{3CFF4FB4-495E-4982-B059-C6B847B23D58}"/>
-    </customSheetView>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{96B3A945-FB99-402E-AFD9-475201AF1BD3}"/>
+      <autoFilter ref="A293:C332" xr:uid="{4A992B84-A4F5-4EF2-8862-DC0C68127786}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -33627,7 +33631,9 @@
   </sheetPr>
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
given pair sum in sorted and rotated array
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFA6185-F996-4646-B5C2-C979B874B5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822A8444-32D7-489E-9C67-94639E3E6F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,8 +2739,8 @@
   </sheetPr>
   <dimension ref="A1:AC914"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3625,7 +3625,9 @@
       <c r="B24" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D24" s="41"/>
       <c r="E24" s="12" t="s">
         <v>48</v>
@@ -33221,21 +33223,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{AA339591-1250-46F1-A629-591C44240F05}"/>
+      <autoFilter ref="A293:C332" xr:uid="{91A09FDF-5229-4587-A9CD-57CE399E3B82}"/>
+    </customSheetView>
+    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{773E2A67-05A0-4258-B0D7-9B8C8F718B71}"/>
     </customSheetView>
     <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{9C473676-C4E1-4CBD-8AA3-2A3E76780763}"/>
+      <autoFilter ref="A11:D37" xr:uid="{B71070BF-636E-474A-9F3E-71DC2631685F}"/>
     </customSheetView>
-    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{13E6EA58-A3C6-438A-9C99-AA00D7C85D36}"/>
-    </customSheetView>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{4A992B84-A4F5-4EF2-8862-DC0C68127786}"/>
+      <autoFilter ref="A11:C37" xr:uid="{33801689-0A08-4022-ADAE-D8794DFA4D15}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
find minimum in rotated and sorted array
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822A8444-32D7-489E-9C67-94639E3E6F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB17E74-77A7-4846-AD8C-2E4FD0C3692B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2740,7 +2740,7 @@
   <dimension ref="A1:AC914"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3475,7 +3475,9 @@
       <c r="B20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D20" s="41"/>
       <c r="E20" s="12" t="s">
         <v>40</v>
@@ -3512,7 +3514,9 @@
       <c r="B21" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="30"/>
+      <c r="C21" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D21" s="42"/>
       <c r="E21" s="12" t="s">
         <v>42</v>
@@ -33223,21 +33227,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{91A09FDF-5229-4587-A9CD-57CE399E3B82}"/>
+      <autoFilter ref="A11:C37" xr:uid="{99DFEB12-0D60-4860-AF36-0A0EC56E2289}"/>
+    </customSheetView>
+    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{9D7F700A-9E7D-452F-85E7-C2C11B11E4FA}"/>
     </customSheetView>
     <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{773E2A67-05A0-4258-B0D7-9B8C8F718B71}"/>
+      <autoFilter ref="A11:D37" xr:uid="{90845E34-C155-47C0-9F57-671DE3DD1D09}"/>
     </customSheetView>
-    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{B71070BF-636E-474A-9F3E-71DC2631685F}"/>
-    </customSheetView>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{33801689-0A08-4022-ADAE-D8794DFA4D15}"/>
+      <autoFilter ref="A293:C332" xr:uid="{808519ED-F074-4098-ACC2-F6F317244E7C}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
search in rotated and sorted array
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB17E74-77A7-4846-AD8C-2E4FD0C3692B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C5DFBC-9AB1-4323-9D4A-E6181C53EB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,8 +2739,8 @@
   </sheetPr>
   <dimension ref="A1:AC914"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3155,7 +3155,9 @@
       <c r="B12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D12" s="40" t="s">
         <v>699</v>
       </c>
@@ -33227,21 +33229,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{99DFEB12-0D60-4860-AF36-0A0EC56E2289}"/>
+      <autoFilter ref="A293:C332" xr:uid="{D2E4F818-0F29-4421-90BC-46435663EAFD}"/>
+    </customSheetView>
+    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{619F39E0-FEBB-4B9E-A07D-5528BD619E1B}"/>
     </customSheetView>
     <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{9D7F700A-9E7D-452F-85E7-C2C11B11E4FA}"/>
+      <autoFilter ref="A11:D37" xr:uid="{8218DBB5-078B-42AB-9440-A8C40FD05A85}"/>
     </customSheetView>
-    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{90845E34-C155-47C0-9F57-671DE3DD1D09}"/>
-    </customSheetView>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{808519ED-F074-4098-ACC2-F6F317244E7C}"/>
+      <autoFilter ref="A11:C37" xr:uid="{86EC24C3-1435-420D-BD35-01B7EE3E83E3}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
container with most water
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C5DFBC-9AB1-4323-9D4A-E6181C53EB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7280BB0-1C6A-45C9-8442-63C424A3C4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,8 +2739,8 @@
   </sheetPr>
   <dimension ref="A1:AC914"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3592,7 +3592,9 @@
       <c r="B23" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D23" s="41"/>
       <c r="E23" s="12" t="s">
         <v>45</v>
@@ -33229,21 +33231,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{D2E4F818-0F29-4421-90BC-46435663EAFD}"/>
+      <autoFilter ref="A11:C37" xr:uid="{985A7681-6F08-4A38-913A-BDCEB9D41AEA}"/>
+    </customSheetView>
+    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{57174448-1A95-4151-A5AC-7E43D57ABD72}"/>
     </customSheetView>
     <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{619F39E0-FEBB-4B9E-A07D-5528BD619E1B}"/>
+      <autoFilter ref="A11:D37" xr:uid="{9E673C28-5E0A-425D-B5B8-70E37D17EC6E}"/>
     </customSheetView>
-    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{8218DBB5-078B-42AB-9440-A8C40FD05A85}"/>
-    </customSheetView>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{86EC24C3-1435-420D-BD35-01B7EE3E83E3}"/>
+      <autoFilter ref="A293:C332" xr:uid="{0FF253DE-B874-4810-B710-0A2F265C02B3}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
product of array except self
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7280BB0-1C6A-45C9-8442-63C424A3C4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB49A8C-456A-4D81-BE9D-7FD7954C0E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,8 +2739,8 @@
   </sheetPr>
   <dimension ref="A1:AC914"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3397,7 +3397,9 @@
       <c r="B18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D18" s="40" t="s">
         <v>699</v>
       </c>
@@ -33231,21 +33233,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{985A7681-6F08-4A38-913A-BDCEB9D41AEA}"/>
+      <autoFilter ref="A293:C332" xr:uid="{761BB238-E391-481E-B8FD-CB0A433B1755}"/>
+    </customSheetView>
+    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{108EF115-845A-4A3B-8052-2A172855A7E8}"/>
     </customSheetView>
     <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{57174448-1A95-4151-A5AC-7E43D57ABD72}"/>
+      <autoFilter ref="A11:D37" xr:uid="{C44F38EF-0C34-44B6-B362-B7899E4F5FAF}"/>
     </customSheetView>
-    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{9E673C28-5E0A-425D-B5B8-70E37D17EC6E}"/>
-    </customSheetView>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{0FF253DE-B874-4810-B710-0A2F265C02B3}"/>
+      <autoFilter ref="A11:C37" xr:uid="{E2E80559-C2F5-4CC9-91F6-8A15A823A0BE}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
repeating and missing number in array
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB49A8C-456A-4D81-BE9D-7FD7954C0E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3A9499-9752-452A-B2D2-91A1243FBD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,8 +2739,8 @@
   </sheetPr>
   <dimension ref="A1:AC914"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3276,7 +3276,9 @@
       <c r="B15" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D15" s="40" t="s">
         <v>699</v>
       </c>
@@ -33233,21 +33235,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{761BB238-E391-481E-B8FD-CB0A433B1755}"/>
+      <autoFilter ref="A11:C37" xr:uid="{18D21E8F-D68F-4802-A7E0-218B7EB2DBCF}"/>
+    </customSheetView>
+    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{88515606-CB09-4FD7-B4F9-1570D280E99B}"/>
     </customSheetView>
     <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{108EF115-845A-4A3B-8052-2A172855A7E8}"/>
+      <autoFilter ref="A11:D37" xr:uid="{E430442E-27AD-4022-B1DB-883F559B6FDE}"/>
     </customSheetView>
-    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{C44F38EF-0C34-44B6-B362-B7899E4F5FAF}"/>
-    </customSheetView>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{E2E80559-C2F5-4CC9-91F6-8A15A823A0BE}"/>
+      <autoFilter ref="A293:C332" xr:uid="{13E5D171-0A15-43E5-8FFA-3D1605DE2F15}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
finding kth largest and kth smallest element in array
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7FCE66-2EC3-42AC-8D22-38FE4D2897AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B646E741-CF78-40E2-8E7D-1D59EB763D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2740,7 +2740,7 @@
   <dimension ref="A1:AC914"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="105" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3678,7 +3678,9 @@
       <c r="B25" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D25" s="40" t="s">
         <v>699</v>
       </c>
@@ -33237,21 +33239,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{293C8795-6939-4E15-B490-FFC01FE455D6}"/>
+      <autoFilter ref="A11:C37" xr:uid="{7BD083F4-5F6C-4FEA-8E6B-74AAA946FDDF}"/>
+    </customSheetView>
+    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{A66C32C1-26F9-421A-B5CD-EA442378FB39}"/>
     </customSheetView>
     <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{598D237A-EC0D-497C-BE05-D9330E3E675A}"/>
+      <autoFilter ref="A11:D37" xr:uid="{D9ACB83B-9FF9-4372-803A-BCCB2815BD1E}"/>
     </customSheetView>
-    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{A0CA90FA-2429-40BC-A251-DEB7926EB804}"/>
-    </customSheetView>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{F28D4393-0909-4E75-A127-38A37EBE53B8}"/>
+      <autoFilter ref="A293:C332" xr:uid="{D714103B-D760-42BD-823C-859E73C4085B}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
create largest concatenated number
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B646E741-CF78-40E2-8E7D-1D59EB763D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9816BCEF-D650-4852-9741-0644EB1F04C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,8 +2739,8 @@
   </sheetPr>
   <dimension ref="A1:AC914"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3319,7 +3319,9 @@
       <c r="B16" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D16" s="40" t="s">
         <v>699</v>
       </c>
@@ -3792,7 +3794,9 @@
       <c r="B28" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="E28" s="12" t="s">
         <v>55</v>
       </c>
@@ -33239,21 +33243,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{7BD083F4-5F6C-4FEA-8E6B-74AAA946FDDF}"/>
+      <autoFilter ref="A293:C332" xr:uid="{403AAA70-4867-44AE-A396-4C945D9324A0}"/>
+    </customSheetView>
+    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{76B72831-92A8-4EC8-A737-6531D6EC8004}"/>
     </customSheetView>
     <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{A66C32C1-26F9-421A-B5CD-EA442378FB39}"/>
+      <autoFilter ref="A11:D37" xr:uid="{CF55B50C-2AF3-45C8-B14B-4FF2E2A1DE28}"/>
     </customSheetView>
-    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{D9ACB83B-9FF9-4372-803A-BCCB2815BD1E}"/>
-    </customSheetView>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{D714103B-D760-42BD-823C-859E73C4085B}"/>
+      <autoFilter ref="A11:C37" xr:uid="{58CBA2C6-A520-44EC-9737-FB8DF8ED064C}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Permute Two Arrays such that Sum of Every Pair is Greater or Equal to K
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A306E7-CAFA-4F71-908E-2ABDA7D43671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3010BBE9-985C-4B74-9BC6-983F79FE22A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,8 +2739,8 @@
   </sheetPr>
   <dimension ref="A1:AC914"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5362,7 +5362,9 @@
       <c r="B71" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C71" s="31"/>
+      <c r="C71" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D71" s="41"/>
       <c r="E71" s="12" t="s">
         <v>129</v>
@@ -33249,21 +33251,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{74CC02F8-A59E-4927-A235-9126A4DCBAA0}"/>
+      <autoFilter ref="A293:C332" xr:uid="{55FA2094-C16B-4512-AB14-7198D61D6896}"/>
+    </customSheetView>
+    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{9D24A30D-46F4-45F5-BCF2-7F097528CF16}"/>
     </customSheetView>
     <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{F1CE6741-F220-498B-B1C8-32AE9F9042B4}"/>
+      <autoFilter ref="A11:D37" xr:uid="{7F36A106-C3E6-4B2B-9EDD-343A51537E36}"/>
     </customSheetView>
-    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{B65F90A1-4B11-4FFF-B7B5-4AA8FDB9E984}"/>
-    </customSheetView>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{88FDFF61-5445-4143-B8D1-04C6AAFD3B9E}"/>
+      <autoFilter ref="A11:C37" xr:uid="{25E286C5-5B55-411E-8DE1-5C6A849E3BED}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
finding common elements in three sorted arrays
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3010BBE9-985C-4B74-9BC6-983F79FE22A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F66E20-D00A-489E-A534-9A3BCC97FEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2740,7 +2740,7 @@
   <dimension ref="A1:AC914"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5438,7 +5438,9 @@
       <c r="B73" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="C73" s="31"/>
+      <c r="C73" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D73" s="41"/>
       <c r="E73" s="12" t="s">
         <v>123</v>
@@ -33251,21 +33253,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{55FA2094-C16B-4512-AB14-7198D61D6896}"/>
+      <autoFilter ref="A11:C37" xr:uid="{7E6BA0A0-0988-400C-963E-D3C2589B70DB}"/>
+    </customSheetView>
+    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{75CA9750-6B30-4C01-8CF3-54A4835F1B0D}"/>
     </customSheetView>
     <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{9D24A30D-46F4-45F5-BCF2-7F097528CF16}"/>
+      <autoFilter ref="A11:D37" xr:uid="{B7C70064-F9B3-4279-9290-543149F2240C}"/>
     </customSheetView>
-    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{7F36A106-C3E6-4B2B-9EDD-343A51537E36}"/>
-    </customSheetView>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{25E286C5-5B55-411E-8DE1-5C6A849E3BED}"/>
+      <autoFilter ref="A293:C332" xr:uid="{896812AA-3C53-4AD8-9FCB-3732DB2250F3}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Searching in an array where adjacent differ by at most k
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F66E20-D00A-489E-A534-9A3BCC97FEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C45AAD7-971F-471A-B05B-3E9441F91C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2740,7 +2740,7 @@
   <dimension ref="A1:AC914"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5477,7 +5477,9 @@
       <c r="B74" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C74" s="31"/>
+      <c r="C74" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D74" s="41"/>
       <c r="E74" s="12" t="s">
         <v>134</v>
@@ -33253,21 +33255,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{7E6BA0A0-0988-400C-963E-D3C2589B70DB}"/>
+      <autoFilter ref="A293:C332" xr:uid="{BE0E08B5-3C4A-4FC2-9237-DC56F34A01FF}"/>
+    </customSheetView>
+    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{6FE80D4C-5A95-41CB-ADBB-4134DEA739DA}"/>
     </customSheetView>
     <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{75CA9750-6B30-4C01-8CF3-54A4835F1B0D}"/>
+      <autoFilter ref="A11:D37" xr:uid="{F9640821-01DC-4292-B117-142DD7784A77}"/>
     </customSheetView>
-    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{B7C70064-F9B3-4279-9290-543149F2240C}"/>
-    </customSheetView>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{896812AA-3C53-4AD8-9FCB-3732DB2250F3}"/>
+      <autoFilter ref="A11:C37" xr:uid="{5895A0E9-0F89-49C4-A5D7-473972E545B5}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
ceiling in sorted array searching and sorting
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C45AAD7-971F-471A-B05B-3E9441F91C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430C8822-8288-4245-B8CD-D213485B6B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,8 +2739,8 @@
   </sheetPr>
   <dimension ref="A1:AC914"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5516,7 +5516,9 @@
       <c r="B75" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="C75" s="31"/>
+      <c r="C75" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D75" s="41"/>
       <c r="E75" s="12" t="s">
         <v>136</v>
@@ -33255,21 +33257,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{BE0E08B5-3C4A-4FC2-9237-DC56F34A01FF}"/>
+      <autoFilter ref="A11:C37" xr:uid="{39E25E32-735D-4BC2-B7A2-4AE8213E59B5}"/>
+    </customSheetView>
+    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{D29DA7B5-C0D7-499C-ABFC-6830DB817164}"/>
     </customSheetView>
     <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{6FE80D4C-5A95-41CB-ADBB-4134DEA739DA}"/>
+      <autoFilter ref="A11:D37" xr:uid="{5033F451-A53E-4F25-B235-A190386B32B1}"/>
     </customSheetView>
-    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{F9640821-01DC-4292-B117-142DD7784A77}"/>
-    </customSheetView>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{5895A0E9-0F89-49C4-A5D7-473972E545B5}"/>
+      <autoFilter ref="A293:C332" xr:uid="{676F2F63-55C9-485F-9799-77E211A2E901}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
pair with given difference searching and sorting
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430C8822-8288-4245-B8CD-D213485B6B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473B12D8-DF8C-46DE-AA3E-0CA50DA6FB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2740,7 +2740,7 @@
   <dimension ref="A1:AC914"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5555,7 +5555,9 @@
       <c r="B76" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="C76" s="31"/>
+      <c r="C76" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D76" s="41"/>
       <c r="E76" s="12" t="s">
         <v>138</v>
@@ -33257,21 +33259,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{39E25E32-735D-4BC2-B7A2-4AE8213E59B5}"/>
+      <autoFilter ref="A293:C332" xr:uid="{F063E7B7-67D0-4539-B8E0-2BB1A71A4426}"/>
+    </customSheetView>
+    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{C7442002-2D04-4764-BC41-E222901A0818}"/>
     </customSheetView>
     <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{D29DA7B5-C0D7-499C-ABFC-6830DB817164}"/>
+      <autoFilter ref="A11:D37" xr:uid="{E39A8A70-66F6-45C3-8633-BD461886AE42}"/>
     </customSheetView>
-    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{5033F451-A53E-4F25-B235-A190386B32B1}"/>
-    </customSheetView>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{676F2F63-55C9-485F-9799-77E211A2E901}"/>
+      <autoFilter ref="A11:C37" xr:uid="{ABB95408-7DF5-4031-A0C3-20DC0DD97B78}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
majority element searching and sorting
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473B12D8-DF8C-46DE-AA3E-0CA50DA6FB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDA3565-509C-4BC5-87F5-5C803168EFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2740,7 +2740,7 @@
   <dimension ref="A1:AC914"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5594,7 +5594,9 @@
       <c r="B77" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="C77" s="32"/>
+      <c r="C77" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D77" s="44"/>
       <c r="E77" s="12" t="s">
         <v>140</v>
@@ -33259,21 +33261,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{F063E7B7-67D0-4539-B8E0-2BB1A71A4426}"/>
+      <autoFilter ref="A11:C37" xr:uid="{1FF6F711-3D34-4FFE-A7E5-D6AE4C4AD7A3}"/>
+    </customSheetView>
+    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{F7D1D9A8-58C5-4C73-9C4C-B1A99E4E0AA3}"/>
     </customSheetView>
     <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{C7442002-2D04-4764-BC41-E222901A0818}"/>
+      <autoFilter ref="A11:D37" xr:uid="{B954E505-2019-47BD-B11F-D3553A0C8112}"/>
     </customSheetView>
-    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{E39A8A70-66F6-45C3-8633-BD461886AE42}"/>
-    </customSheetView>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{ABB95408-7DF5-4031-A0C3-20DC0DD97B78}"/>
+      <autoFilter ref="A293:C332" xr:uid="{27232AC9-74CE-4C2A-8FD5-EC36CF194FD9}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
count triplets with sum smaller than value given searching and sorting
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aryan_Mule\OneDrive\Desktop\DSA\DSA-Practitioner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDA3565-509C-4BC5-87F5-5C803168EFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFE5729-A021-4A35-9E6B-27DB251B541A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2740,7 +2740,7 @@
   <dimension ref="A1:AC914"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5633,7 +5633,9 @@
       <c r="B78" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="C78" s="32"/>
+      <c r="C78" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="D78" s="44"/>
       <c r="E78" s="12" t="s">
         <v>142</v>
@@ -33261,21 +33263,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{1FF6F711-3D34-4FFE-A7E5-D6AE4C4AD7A3}"/>
+      <autoFilter ref="A293:C332" xr:uid="{3FDCEEBD-81F6-467F-A74F-EACD27AD5F8C}"/>
+    </customSheetView>
+    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{D990F9CF-3DBA-4942-B865-6FC33D74E8CD}"/>
     </customSheetView>
     <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{F7D1D9A8-58C5-4C73-9C4C-B1A99E4E0AA3}"/>
+      <autoFilter ref="A11:D37" xr:uid="{2FF2D49F-F7C9-4A64-B2D3-878750EC5A49}"/>
     </customSheetView>
-    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{B954E505-2019-47BD-B11F-D3553A0C8112}"/>
-    </customSheetView>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{27232AC9-74CE-4C2A-8FD5-EC36CF194FD9}"/>
+      <autoFilter ref="A11:C37" xr:uid="{A18603A0-0B7E-49A1-A2F3-2C79FA03B9B1}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>